<commit_message>
remove redundant waits from file
</commit_message>
<xml_diff>
--- a/testData/bluenile.xlsx
+++ b/testData/bluenile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/ZS_Playwright_GenAI/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="6_{7FD022CF-C216-4189-B51E-8EC99E25A265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7157CBA3-60FB-4EE6-AD3A-F0F1FB1B71EE}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="6_{7FD022CF-C216-4189-B51E-8EC99E25A265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A4563B8-E6E2-4270-A6B3-B0B5D6137300}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
   <si>
     <t>action</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Summary</t>
   </si>
   <si>
-    <t>Book Now button on popup</t>
-  </si>
-  <si>
     <t>We Accept</t>
   </si>
   <si>
@@ -129,7 +126,16 @@
     <t>Phone Number input field</t>
   </si>
   <si>
-    <t>Zip / Postal Code</t>
+    <t>Contact information</t>
+  </si>
+  <si>
+    <t>assert</t>
+  </si>
+  <si>
+    <t>section[data-qa="step_box-user_authentication_step-checkout_page"]&gt;div&gt;address</t>
+  </si>
+  <si>
+    <t>Use same address for billing</t>
   </si>
 </sst>
 </file>
@@ -465,9 +471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -564,7 +568,7 @@
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="1">
@@ -579,7 +583,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1">
         <v>1000</v>
@@ -590,16 +594,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E9" s="1">
-        <v>5000</v>
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -607,21 +605,30 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1">
         <v>1000</v>
       </c>
       <c r="E10" s="1">
-        <v>5000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2000</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -629,30 +636,21 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1">
         <v>1000</v>
       </c>
       <c r="E12" s="1">
-        <v>2000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E13" s="1">
-        <v>2000</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -660,21 +658,30 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D14" s="1">
         <v>1000</v>
       </c>
       <c r="E14" s="1">
-        <v>5000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2000</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -682,7 +689,7 @@
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D16" s="1">
         <v>1000</v>
@@ -693,13 +700,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1">
         <v>1000</v>
@@ -713,7 +720,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1">
         <v>1000</v>
@@ -724,27 +731,27 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D19" s="1">
         <v>1000</v>
       </c>
       <c r="E19" s="1">
-        <v>2000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D20" s="1">
         <v>1000</v>
@@ -755,27 +762,27 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="D21" s="1">
         <v>1000</v>
       </c>
       <c r="E21" s="1">
-        <v>3000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D22" s="1">
         <v>1000</v>
@@ -786,12 +793,9 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D23" s="1">
@@ -803,10 +807,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="C24" s="1">
+        <v>6142273098</v>
       </c>
       <c r="D24" s="1">
         <v>1000</v>
@@ -820,7 +827,7 @@
         <v>7</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D25" s="1">
         <v>1000</v>
@@ -831,14 +838,11 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="1">
-        <v>6142273098</v>
-      </c>
       <c r="D26" s="1">
         <v>1000</v>
       </c>
@@ -848,10 +852,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>21</v>
+        <v>35</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D27" s="1">
         <v>1000</v>
@@ -860,9 +867,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{979FC2DF-A930-4714-8BCF-A210590BEE43}"/>
-    <hyperlink ref="C13" r:id="rId2" xr:uid="{5A356B78-98B4-49E8-BE22-9B36B0131DAC}"/>
+    <hyperlink ref="C11" r:id="rId2" xr:uid="{5A356B78-98B4-49E8-BE22-9B36B0131DAC}"/>
+    <hyperlink ref="C27" r:id="rId3" xr:uid="{5B1FC407-A0DF-4B94-9734-7DD4AE86FF58}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implemented multiple test case execution
</commit_message>
<xml_diff>
--- a/testData/bluenile.xlsx
+++ b/testData/bluenile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/ZS_Playwright_GenAI/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="6_{7FD022CF-C216-4189-B51E-8EC99E25A265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B56720A-4CE5-41A0-BDD9-5F771A406CD6}"/>
+  <xr:revisionPtr revIDLastSave="143" documentId="6_{7FD022CF-C216-4189-B51E-8EC99E25A265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF78FC8A-0E2D-49A6-85BD-95CF66D4B975}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>action</t>
   </si>
@@ -83,31 +83,37 @@
     <t>We Accept</t>
   </si>
   <si>
-    <t>Checkout button</t>
-  </si>
-  <si>
-    <t>Please provide an email address</t>
-  </si>
-  <si>
-    <t>Email Address input field</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>mellina@gmail.com</t>
-  </si>
-  <si>
-    <t>Continue button</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
     <t>assert</t>
   </si>
   <si>
-    <t>#deliveryParser,email</t>
+    <t>TestID</t>
+  </si>
+  <si>
+    <t>TC001</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/</t>
+  </si>
+  <si>
+    <t>waitfortext</t>
+  </si>
+  <si>
+    <t>Hello, Sign in</t>
+  </si>
+  <si>
+    <t>span#nav-link-accountList-nav-line-1</t>
+  </si>
+  <si>
+    <t>Automation</t>
   </si>
 </sst>
 </file>
@@ -441,219 +447,222 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="21.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="3" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="21.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1">
+      <c r="F2" s="1">
         <v>1000</v>
       </c>
-      <c r="E2" s="1">
+      <c r="G2" s="1">
         <v>9000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1">
+      <c r="F3" s="1">
         <v>1000</v>
       </c>
-      <c r="E3" s="1">
+      <c r="G3" s="1">
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1">
+      <c r="F4" s="1">
         <v>1000</v>
       </c>
-      <c r="E4" s="1">
+      <c r="G4" s="1">
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1">
+      <c r="F5" s="1">
         <v>1000</v>
       </c>
-      <c r="E5" s="1">
+      <c r="G5" s="1">
         <v>9000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="1">
+      <c r="F7" s="1">
         <v>1000</v>
       </c>
-      <c r="E7" s="1">
+      <c r="G7" s="1">
         <v>5000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G8" s="1">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="1">
         <v>1000</v>
       </c>
-      <c r="E8" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E10" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E11" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E12" s="1">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="1">
-        <v>2000</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C27" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E26" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{979FC2DF-A930-4714-8BCF-A210590BEE43}"/>
-    <hyperlink ref="C11" r:id="rId2" xr:uid="{5A356B78-98B4-49E8-BE22-9B36B0131DAC}"/>
-    <hyperlink ref="C14" r:id="rId3" xr:uid="{7EE9AC3C-2E60-4275-B19A-60AA1393C51C}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{979FC2DF-A930-4714-8BCF-A210590BEE43}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AI as an alternative approach to traditional item locators
</commit_message>
<xml_diff>
--- a/testData/bluenile.xlsx
+++ b/testData/bluenile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://talentkloud-my.sharepoint.com/personal/vaibhav_gangrade_codvo_ai/Documents/Documents/Codvo.ai/MyProject/ZS_Playwright_GenAI/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="6_{7FD022CF-C216-4189-B51E-8EC99E25A265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF78FC8A-0E2D-49A6-85BD-95CF66D4B975}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="6_{7FD022CF-C216-4189-B51E-8EC99E25A265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B474917-2A8B-40D7-8F61-6976D4624840}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>action</t>
   </si>
@@ -59,15 +59,9 @@
     <t>scroll</t>
   </si>
   <si>
-    <t>click</t>
-  </si>
-  <si>
     <t>https://www.bluenile.com/shopping-cart</t>
   </si>
   <si>
-    <t>ADD TO CART button</t>
-  </si>
-  <si>
     <t>https://www.bluenile.com/jewelry/necklaces/lab-grown-diamond-cushion-cut-solitaire-pendant-in-14k-white-gold-1-2-ct-tw-f-g-vs2-si1-item-202314</t>
   </si>
   <si>
@@ -83,9 +77,6 @@
     <t>We Accept</t>
   </si>
   <si>
-    <t>assert</t>
-  </si>
-  <si>
     <t>TestID</t>
   </si>
   <si>
@@ -95,9 +86,6 @@
     <t>Enabled</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>TC002</t>
   </si>
   <si>
@@ -110,10 +98,28 @@
     <t>Hello, Sign in</t>
   </si>
   <si>
-    <t>span#nav-link-accountList-nav-line-1</t>
-  </si>
-  <si>
-    <t>Automation</t>
+    <t>textclick</t>
+  </si>
+  <si>
+    <t>locatorType</t>
+  </si>
+  <si>
+    <t>ADD TO CART</t>
+  </si>
+  <si>
+    <t>button</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>div</t>
+  </si>
+  <si>
+    <t>Sign in</t>
   </si>
 </sst>
 </file>
@@ -447,26 +453,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="21.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="5" width="21.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -475,188 +483,213 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="G2" s="1">
         <v>1000</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>9000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1">
         <v>1000</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1">
         <v>1000</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1">
+        <v>7</v>
+      </c>
+      <c r="G5" s="1">
         <v>1000</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>9000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="1">
+        <v>12</v>
+      </c>
+      <c r="E7"/>
+      <c r="G7" s="1">
         <v>1000</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>5000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="1">
+        <v>17</v>
+      </c>
+      <c r="G8" s="1">
         <v>1000</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>5000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="E10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="1">
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="1">
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E13" s="2"/>
-    </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E26" s="2"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F26" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>